<commit_message>
updated corresponding reference file
</commit_message>
<xml_diff>
--- a/src/zdemo_excel3.w3mi.data.xlsx
+++ b/src/zdemo_excel3.w3mi.data.xlsx
@@ -438,7 +438,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" zoomScaleSheetLayoutView="100" workbookViewId="0" showGridLines="1" showRowColHeaders="1">
-      <pane ySplit="3" xSplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane ySplit="1" xSplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1486,7 +1486,7 @@
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="0" showInputMessage="1" showErrorMessage="1" ShowDropDown="0" errorStyle="stop" sqref="C4">
+    <dataValidation type="list" allowBlank="0" showInputMessage="1" showErrorMessage="1" ShowDropDown="0" errorStyle="stop" sqref="A1:A1048576">
       <formula1>Airlines</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>